<commit_message>
git中.gitignore文件对.idea无效的解决方法 Signed-off-by: componey_qss <475185283@qq.com>
</commit_message>
<xml_diff>
--- a/code_manage/git/gitignore-忽略文件.xlsx
+++ b/code_manage/git/gitignore-忽略文件.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0D80A8A-13BD-4D39-9A7A-F4711348A01C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="25080" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,15 +19,62 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>.gitignore对.idea文件忽略没效果</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在.idea文件目录运行git.bash</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>git rm -r --cached .idea/*</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>上句代码会删除掉缓存中的.idea下所有文件，实际目录没有</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>按改动文件正常提交到origin/master</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在.gitignore文件中添加.idea并提交到origin/master即可</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>【原因就是git已经关联追踪了这些文件，再次设置ignore时无效。需要执行一次 git rm -r --cached 目录名称/文件名称】</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -49,11 +97,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -330,13 +382,98 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A46:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51:G51"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="41.25" defaultRowHeight="22.5" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="41.25" style="1"/>
+    <col min="2" max="2" width="8.75" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="41.25" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A46" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C47" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="C48" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+    </row>
+    <row r="49" spans="3:9" x14ac:dyDescent="0.4">
+      <c r="C49" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+    </row>
+    <row r="50" spans="3:9" x14ac:dyDescent="0.4">
+      <c r="C50" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+    </row>
+    <row r="51" spans="3:9" x14ac:dyDescent="0.4">
+      <c r="C51" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="C46:I46"/>
+    <mergeCell ref="C47:I47"/>
+    <mergeCell ref="C48:I48"/>
+    <mergeCell ref="C49:I49"/>
+    <mergeCell ref="C50:I50"/>
+    <mergeCell ref="C51:G51"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>